<commit_message>
Actualización: nuevos modelos, reportes PDF/Excel, tabla editable, roles y observaciones
</commit_message>
<xml_diff>
--- a/static/plantillas/plantilla_personal.xlsx
+++ b/static/plantillas/plantilla_personal.xlsx
@@ -1,95 +1,182 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CD\static\plantillas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1609B0F-06BD-4C76-8301-9CF02B96E299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>apellido_paterno</t>
-  </si>
-  <si>
-    <t>apellido_materno</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>genero</t>
-  </si>
-  <si>
-    <t>rfc</t>
-  </si>
-  <si>
-    <t>curp</t>
-  </si>
-  <si>
-    <t>clave_presupuestal</t>
-  </si>
-  <si>
-    <t>funcion</t>
-  </si>
-  <si>
-    <t>grado_maximo_estudios</t>
-  </si>
-  <si>
-    <t>titulado</t>
-  </si>
-  <si>
-    <t>fecha_ingreso</t>
-  </si>
-  <si>
-    <t>fecha_baja_jubilacion</t>
-  </si>
-  <si>
-    <t>estatus_membresia</t>
-  </si>
-  <si>
-    <t>nombramiento</t>
-  </si>
-  <si>
-    <t>domicilio</t>
-  </si>
-  <si>
-    <t>numero</t>
-  </si>
-  <si>
-    <t>localidad</t>
-  </si>
-  <si>
-    <t>colonia</t>
-  </si>
-  <si>
-    <t>municipio</t>
-  </si>
-  <si>
-    <t>cp</t>
-  </si>
-  <si>
-    <t>tel1</t>
-  </si>
-  <si>
-    <t>tel2</t>
-  </si>
-  <si>
-    <t>correo_electronico</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+  <si>
+    <t>NUM</t>
+  </si>
+  <si>
+    <t>PATERNO</t>
+  </si>
+  <si>
+    <t>MATERNO</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>GENERO</t>
+  </si>
+  <si>
+    <t>RFC</t>
+  </si>
+  <si>
+    <t>CURP</t>
+  </si>
+  <si>
+    <t>CLAVE_PRESUPUESTAL</t>
+  </si>
+  <si>
+    <t>FUNCION</t>
+  </si>
+  <si>
+    <t>GRADO_MAXIMO_ESTUDIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TITULADO </t>
+  </si>
+  <si>
+    <t>FECHA_INGRESO</t>
+  </si>
+  <si>
+    <t>FCH_BAJ_JUB</t>
+  </si>
+  <si>
+    <t>STATUS_MEMB</t>
+  </si>
+  <si>
+    <t>NOMBRAMIENTO</t>
+  </si>
+  <si>
+    <t>DP_CALLE</t>
+  </si>
+  <si>
+    <t>DP_NUM_EXT</t>
+  </si>
+  <si>
+    <t>DP_NUM_INT</t>
+  </si>
+  <si>
+    <t>DP_CRUCE1</t>
+  </si>
+  <si>
+    <t>DP_CRUCE2</t>
+  </si>
+  <si>
+    <t>DP_LOCALIDAD</t>
+  </si>
+  <si>
+    <t>DP_COLONIA</t>
+  </si>
+  <si>
+    <t>DP_MUN_NOM</t>
+  </si>
+  <si>
+    <t>DP_CP</t>
+  </si>
+  <si>
+    <t>DP_TEL1</t>
+  </si>
+  <si>
+    <t>DP_TEL2</t>
+  </si>
+  <si>
+    <t>CORREO_ELECTRONICO</t>
+  </si>
+  <si>
+    <t>ESCUELA_NOMBRE</t>
+  </si>
+  <si>
+    <t>CCT</t>
+  </si>
+  <si>
+    <t>TURNO</t>
+  </si>
+  <si>
+    <t>NIVEL</t>
+  </si>
+  <si>
+    <t>SUBS_MODALIDAD</t>
+  </si>
+  <si>
+    <t>ZONA_ESCOLAR</t>
+  </si>
+  <si>
+    <t>SECTOR</t>
+  </si>
+  <si>
+    <t>DOM_ESC_CALLE</t>
+  </si>
+  <si>
+    <t>DOM_ESC_NUM_EXT</t>
+  </si>
+  <si>
+    <t>DOM_ESC_NUM_INT</t>
+  </si>
+  <si>
+    <t>DOM_ESC_CRUCE1</t>
+  </si>
+  <si>
+    <t>DOM_ESC_CRUCE2</t>
+  </si>
+  <si>
+    <t>DOM_ESC_LOCALIDAD</t>
+  </si>
+  <si>
+    <t>DOM_ESC_COLONIA</t>
+  </si>
+  <si>
+    <t>DOM_ESC_MUN_NOM</t>
+  </si>
+  <si>
+    <t>DOM_ESC_CP</t>
+  </si>
+  <si>
+    <t>DOM_ESC_COORDENADAS GPS</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>SECCION_SNTE</t>
+  </si>
+  <si>
+    <t>DEL_O_CT</t>
+  </si>
+  <si>
+    <t>ORG</t>
+  </si>
+  <si>
+    <t>COORD_REG</t>
+  </si>
+  <si>
+    <t>FUN_SIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,15 +190,38 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -141,10 +251,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -152,13 +298,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -196,7 +350,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -230,6 +384,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -264,9 +419,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,82 +595,208 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AX1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="32.5546875" customWidth="1"/>
+    <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
+    <col min="12" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="20.33203125" customWidth="1"/>
+    <col min="16" max="16" width="69.44140625" customWidth="1"/>
+    <col min="17" max="18" width="13.33203125" customWidth="1"/>
+    <col min="19" max="21" width="20.33203125" customWidth="1"/>
+    <col min="22" max="22" width="26" customWidth="1"/>
+    <col min="23" max="23" width="20.33203125" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" customWidth="1"/>
+    <col min="25" max="26" width="20.33203125" customWidth="1"/>
+    <col min="27" max="27" width="50.44140625" customWidth="1"/>
+    <col min="28" max="28" width="41.5546875" customWidth="1"/>
+    <col min="29" max="29" width="26.6640625" customWidth="1"/>
+    <col min="30" max="30" width="18.5546875" customWidth="1"/>
+    <col min="31" max="31" width="23.88671875" customWidth="1"/>
+    <col min="32" max="32" width="23.6640625" customWidth="1"/>
+    <col min="33" max="33" width="14.88671875" customWidth="1"/>
+    <col min="34" max="34" width="14.5546875" customWidth="1"/>
+    <col min="35" max="35" width="21.88671875" customWidth="1"/>
+    <col min="36" max="36" width="14.6640625" customWidth="1"/>
+    <col min="37" max="37" width="14.88671875" customWidth="1"/>
+    <col min="38" max="42" width="19.33203125" customWidth="1"/>
+    <col min="43" max="43" width="12" customWidth="1"/>
+    <col min="44" max="44" width="31.33203125" customWidth="1"/>
+    <col min="45" max="45" width="19.109375" customWidth="1"/>
+    <col min="46" max="46" width="15.33203125" customWidth="1"/>
+    <col min="47" max="47" width="16.33203125" customWidth="1"/>
+    <col min="48" max="48" width="19.5546875" customWidth="1"/>
+    <col min="49" max="49" width="28.33203125" customWidth="1"/>
+    <col min="50" max="50" width="30.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:50" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>